<commit_message>
Sync data files - 2025-07-05 11:01:02 (       1 files updated)
</commit_message>
<xml_diff>
--- a/Data/Layout Types/Maple_layouts.xlsx
+++ b/Data/Layout Types/Maple_layouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levan/Documents/MegaValuationer/Data/Layout Types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDE10AE-14B1-D943-BA31-1E360DB54B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC02C9-9112-7E49-A2EA-D93CB7FD11FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{1FD56F26-AD29-6545-B88A-C8A52BFCC1E6}"/>
   </bookViews>
@@ -43687,7 +43687,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43741,7 +43741,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="3">
-        <v>2228</v>
+        <v>2251</v>
       </c>
       <c r="G2" t="s">
         <v>654</v>
@@ -43787,7 +43787,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="3">
-        <v>2387</v>
+        <v>2406</v>
       </c>
       <c r="G4" t="s">
         <v>654</v>
@@ -43810,7 +43810,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="3">
-        <v>2700</v>
+        <v>2461</v>
       </c>
       <c r="G5" t="s">
         <v>654</v>
@@ -43833,7 +43833,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="3">
-        <v>2228</v>
+        <v>2250</v>
       </c>
       <c r="G6" t="s">
         <v>654</v>
@@ -43879,7 +43879,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="3">
-        <v>2387</v>
+        <v>2406</v>
       </c>
       <c r="G8" t="s">
         <v>654</v>
@@ -43902,7 +43902,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="3">
-        <v>2700</v>
+        <v>2734</v>
       </c>
       <c r="G9" t="s">
         <v>654</v>
@@ -43925,7 +43925,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="3">
-        <v>2228</v>
+        <v>2277</v>
       </c>
       <c r="G10" t="s">
         <v>654</v>
@@ -43948,7 +43948,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="3">
-        <v>2462</v>
+        <v>2500</v>
       </c>
       <c r="G11" t="s">
         <v>654</v>
@@ -43971,7 +43971,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="3">
-        <v>2387</v>
+        <v>2446</v>
       </c>
       <c r="G12" t="s">
         <v>654</v>
@@ -43994,7 +43994,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="3">
-        <v>2700</v>
+        <v>2768</v>
       </c>
       <c r="G13" t="s">
         <v>654</v>

</xml_diff>

<commit_message>
Sync data files - 2025-07-05 11:03:08 (       1 files updated)
</commit_message>
<xml_diff>
--- a/Data/Layout Types/Maple_layouts.xlsx
+++ b/Data/Layout Types/Maple_layouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levan/Documents/MegaValuationer/Data/Layout Types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC02C9-9112-7E49-A2EA-D93CB7FD11FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E802C4-5E99-A24C-96A3-6C47D815DD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{1FD56F26-AD29-6545-B88A-C8A52BFCC1E6}"/>
   </bookViews>
@@ -43687,7 +43687,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43810,7 +43810,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="3">
-        <v>2461</v>
+        <v>2734</v>
       </c>
       <c r="G5" t="s">
         <v>654</v>

</xml_diff>

<commit_message>
Sync data files - 2025-07-06 15:54:00 (       5 files updated)
</commit_message>
<xml_diff>
--- a/Data/Layout Types/Maple_layouts.xlsx
+++ b/Data/Layout Types/Maple_layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levan/Documents/MegaValuationer/Data/Layout Types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E802C4-5E99-A24C-96A3-6C47D815DD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF3C0F0-39EC-994F-8F2C-C1369E0D2EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{1FD56F26-AD29-6545-B88A-C8A52BFCC1E6}"/>
+    <workbookView xWindow="480" yWindow="-19820" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{1FD56F26-AD29-6545-B88A-C8A52BFCC1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11317" uniqueCount="1893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11317" uniqueCount="1896">
   <si>
     <t>Layout Type</t>
   </si>
@@ -5719,6 +5719,15 @@
   </si>
   <si>
     <t>Maple 3</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Subcommunity</t>
   </si>
 </sst>
 </file>
@@ -43687,7 +43696,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43703,13 +43712,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1885</v>
+        <v>1893</v>
       </c>
       <c r="B1" t="s">
-        <v>1886</v>
+        <v>1894</v>
       </c>
       <c r="C1" t="s">
-        <v>1887</v>
+        <v>1895</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>

</xml_diff>